<commit_message>
Changement de theme+voir tableau
-Changement de theme (enfin) oppérationel

-On peut maintenant voir le tableau excel après sa modification
</commit_message>
<xml_diff>
--- a/value.xlsx
+++ b/value.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8505" windowWidth="18195" xWindow="480" yWindow="60"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -120,39 +120,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="4" fillId="3" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="4" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -521,11 +521,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14.14785714285714" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="14.14785714285714" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="8" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="8" width="14.14785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -537,7 +537,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="1">
       <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
@@ -545,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="1">
       <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="4" s="1">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="5" s="1">
       <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
@@ -569,7 +569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="6" s="1">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="1">
       <c r="A7" s="6" t="n">
         <v>5</v>
       </c>
@@ -585,7 +585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="8" s="1">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
@@ -593,7 +593,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="9" s="1">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
@@ -601,7 +601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="15.75" r="10" s="1">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
@@ -610,7 +610,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -628,14 +628,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14.14785714285714" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
-    <col width="14.14785714285714" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="8" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="8" width="14.14785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>air</t>
+          <t>eau</t>
         </is>
       </c>
       <c r="B1" s="3" t="inlineStr">
@@ -644,7 +644,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="2" s="1">
       <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="3" s="1">
       <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="4" s="1">
       <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
@@ -668,7 +668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="5" s="1">
       <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
@@ -676,7 +676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="6" s="1">
       <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
@@ -684,7 +684,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="7" s="1">
       <c r="A7" s="6" t="n">
         <v>5</v>
       </c>
@@ -692,7 +692,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="8" s="1">
       <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
@@ -700,7 +700,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="9" s="1">
       <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
@@ -708,7 +708,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="10" ht="21.75" customFormat="1" customHeight="1" s="1">
+    <row customFormat="1" customHeight="1" ht="21.75" r="10" s="1">
       <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
@@ -717,6 +717,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>